<commit_message>
updated malaya and techtravelmonitor
</commit_message>
<xml_diff>
--- a/pages/fetcher_temp/temp.xlsx
+++ b/pages/fetcher_temp/temp.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -57,13 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,782 +451,3555 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>45589</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Klook celebrates 10 years with biggest travel sale of the decade</t>
+          <t xml:space="preserve"> P12B township to rise in Bacolod City</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/24/klook-celebrates-10-years-with-biggest-travel-sale-of-the-decade/</t>
+          <t>https://malaya.com.ph/special-sections/property/p12b-township-to-rise-in-bacolod-city/</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>45589</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ampverse rolls out next-gen marketing  agency</t>
+          <t>A developer for good</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/24/ampverse-rolls-out-next-gen-market-agency/</t>
+          <t>https://malaya.com.ph/special-sections/property/a-developer-for-good/</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>45588</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PLDT secures P2B loan to expand fiber network</t>
+          <t>SM footprint in Clark: Integrated dev’t exemplified</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/23/pldt-secures-p2b-loan-to-expand-fiber-network/</t>
+          <t>https://malaya.com.ph/special-sections/property/sm-footprint-in-clark-integrated-devt-exemplified/</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>45588</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Gov’t working on ‘abduction’ of American vlogger in Zamboanga</t>
+          <t>8 Filipino projects make it to WAF 2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/23/govt-working-on-abduction-of-american-vlogger-in-zamboanga/</t>
+          <t>https://malaya.com.ph/special-sections/property/8-filipino-projects-make-it-to-waf-2024/</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>45587</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>What are the top Philippine hotels and resorts included in the latest Michelin Guide?</t>
+          <t>Damosa Land marks 20 years of transforming Mindanao real estate</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/22/what-are-the-top-philippine-hotels-and-resorts-included-in-the-michelin-guide/</t>
+          <t>https://malaya.com.ph/special-sections/property/damosa-land-marks-20-years-of-transforming-mindanao-real-estate/</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n">
-        <v>45586</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Israel Ministry of Tourism sees Philippines as key Asian market</t>
+          <t>Massive flooding hits Bicol region</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/21/israel-ministry-of-tourism-sees-philippines-as-key-asian-market/</t>
+          <t>https://malaya.com.ph/news/national-news/massive-flooding-hits-bicol-region/</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n">
-        <v>45586</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Barcode adoption pushed; PH emerges as top source of counterfeit meds</t>
+          <t>Marcos wants use of EDCA sites for storm relief efforts</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/21/barcode-adoption-pushed-ph-emerges-as-top-source-of-counterfeit-meds/</t>
+          <t>https://malaya.com.ph/news/national-news/marcos-wants-use-of-edca-sites-for-storm-relief-efforts/</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="n">
-        <v>45586</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MVP to  CIOs: Handle data wisely, use it for good</t>
+          <t>Quiboloy, accusers face off at Senate hearing</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/21/mvp-to-cios-handle-data-wisely-use-it-for-good/</t>
+          <t>https://malaya.com.ph/news/national-news/quiboloy-accusers-face-off-at-senate-hearing/</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>45585</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>For ePLDT, peace of mind is the ultimate goal of cybersecurity</t>
+          <t>Heeding Sara’s call, Pulong, Migs take drug tests</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/20/for-epldt-peace-of-mind-is-the-ultimate-goal-of-cybersecurity/</t>
+          <t>https://malaya.com.ph/news/national-news/heeding-saras-call-pulong-migs-take-drug-tests/</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n">
-        <v>45585</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7 things to expect with NAIA’s new management</t>
+          <t>Ex-Napolcom exec confirms drug war rewards system</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/20/7-things-to-expect-with-naias-new-management/</t>
+          <t>https://malaya.com.ph/news/national-news/ex-napolcom-exec-confirms-drug-war-rewards-system/</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n">
-        <v>45584</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Study says 98% of PH companies have sustainability targets</t>
+          <t>Angara: Public school teachers play vital role in economic thrust</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/19/study-says-98-of-ph-companies-have-sustainability-targets/</t>
+          <t>https://malaya.com.ph/news/national-news/angara-public-school-teachers-play-vital-role-in-economic-thrust/</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="n">
-        <v>45583</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Digido lends a hand to Rizal’s Cuyambay Elementary School</t>
+          <t>PNP backs plan to reduce number of generals</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/18/digido-lends-a-hand-to-rizals-cuyambay-elementary-school/</t>
+          <t>https://malaya.com.ph/news/national-news/pnp-backs-plan-to-reduce-number-of-generals/</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n">
-        <v>45583</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Smart expands network in Cebu to boost tourism</t>
+          <t>Filipina victim of surrogacy ring barred from boarding flight</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/18/smart-expands-network-in-cebu-to-boost-tourism/</t>
+          <t>https://malaya.com.ph/news/national-news/filipina-victim-of-surrogacy-ring-barred-from-boarding-flight/</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="n">
-        <v>45582</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hong Kong Wine &amp; Dine Festival returns</t>
+          <t>PCO condemns killing of broadcaster in Zamboanga City</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/17/hong-kong-wine-dine-festival-returns/</t>
+          <t>https://malaya.com.ph/news/national-news/pco-condemns-killing-of-broadcaster-in-zamboanga-city/</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="n">
-        <v>45582</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Kaspersky intros solutions to secure industrial firms</t>
+          <t>Migrante calls on new Indonesian president to free Veloso</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/17/kaspersky-intros-solutions-to-secure-industrial-firms/</t>
+          <t>https://malaya.com.ph/news/national-news/migrante-calls-on-new-indonesian-president-to-free-veloso/</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="n">
-        <v>45581</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Filipino startup seeks to map human behavior with AI</t>
+          <t>Moon sample talks show space engagement by rivals US, China</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/16/filipino-startup-seeks-to-map-human-behavior-with-ai/</t>
+          <t>https://malaya.com.ph/news/international-news/moon-sample-talks-show-space-engagement-by-rivals-us-china/</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="n">
-        <v>45581</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PLDT pushes for connectivity in all state universities by 2025</t>
+          <t>Comelec set to file poll offense case vs Guo</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/16/pldt-pushes-for-connectivity-in-all-state-universities-by-2025/</t>
+          <t>https://malaya.com.ph/news/national-news/comelec-set-to-file-poll-offense-case-vs-guo/</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="n">
-        <v>45581</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>The rise of AI agents in the workplace</t>
+          <t>7 Chinese, 1 Vietnamese scammers arrested in Muntinlupa</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/16/the-rise-of-ai-agents-in-the-workplace/</t>
+          <t>https://malaya.com.ph/news/national-news/7-chinese-1-vietnamese-scammers-arrested-in-muntinlupa/</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="n">
-        <v>45580</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>How are influencers shaping Southeast Asia’s e-commerce landscape?</t>
+          <t>Supplier’s P14M claim vs. AFP Health Service Command granted</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/15/how-are-influencers-shaping-southeast-asias-e-commerce-landscape/</t>
+          <t>https://malaya.com.ph/news/national-news/suppliers-p14m-claim-vs-afp-health-service-command-granted/</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="n">
-        <v>45580</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Japan vows to support Philippine cybersecurity efforts</t>
+          <t>P20.4M shabu seized in Zamboanga City; dealer nabbed</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/15/japan-vows-to-support-philippine-cybersecurity/</t>
+          <t>https://malaya.com.ph/news/national-news/p20-4m-shabu-seized-in-zamboanga-city-dealer-nabbed/</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="n">
-        <v>45579</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Transparency is key for Filipino startups, inDrive says</t>
+          <t>7 Vietnamese rescued from trafficking syndicate</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/14/transparency-is-key-for-filipino-startups-indrive-says/</t>
+          <t>https://malaya.com.ph/news/national-news/7-vietnamese-rescued-from-trafficking-syndicate/</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="n">
-        <v>45579</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Converge collaborates with Netflix on streaming bundle</t>
+          <t>Chinese kidnapped in Bulacan released in Manila</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/14/converge-collaborates-with-netflix-on-streaming-bundle/</t>
+          <t>https://malaya.com.ph/news/national-news/chinese-kidnapped-in-bulacan-released-in-manila/</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="n">
-        <v>45579</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>New NAIA rules seek to discourage ‘VIP’ misuse</t>
+          <t>5 killed in firefight in Lanao del Norte</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/14/new-naia-rules-seek-to-discourage-vip-misuse/</t>
+          <t>https://malaya.com.ph/news/national-news/5-killed-in-firefight-in-lanao-del-norte/</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="n">
-        <v>45578</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Globe teams up with Blacklist International; unveils prepaid promo for gamers</t>
+          <t>Cassy Ong cited in contempt anew; detention at correctional jail extended</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/13/globe-teams-up-with-blacklist-international-unveils-prepaid-promo-for-gamers/</t>
+          <t>https://malaya.com.ph/news/national-news/cassy-ong-cited-in-contempt-anew-detention-at-correctional-jail-extended/</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="n">
-        <v>45578</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Bossjob introduces AI Photo Generator to help job seekers</t>
+          <t>DOF execs acquitted on multiple corruption charges</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/13/bossjob-introduces-ai-photo-generator-to-help-job-seekers/</t>
+          <t>https://malaya.com.ph/news/national-news/dof-execs-acquitted-on-multiple-corruption-charges/</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="n">
-        <v>45577</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Adjust unveils multi-platform solution for mobile app marketers</t>
+          <t>Comelec to allow 2025 run of execs with pending appeals of their DQs</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/12/adjust-unveils-multi-platform-solution-for-mobile-app-marketers/</t>
+          <t>https://malaya.com.ph/news/national-news/comelec-to-allow-2025-run-of-execs-with-pending-appeals-of-their-dqs/</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="n">
-        <v>45577</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Globe warns customers vs fraudsters pretending to be NTC officials</t>
+          <t>FPJ Panday Bayanihan: Inclusivity programs for PWDs vital for social progress</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/12/globe-warns-customers-vs-fraudsters-pretending-to-be-ntc-officials/</t>
+          <t>https://malaya.com.ph/news/national-news/fpj-panday-bayanihan-inclusivity-programs-for-pwds-vital-for-social-progress/</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="n">
-        <v>45576</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>UTOL focuses on driver benefits, safety</t>
+          <t>Blinken urges halt to Middle East conflict as Israel bombs historic Lebanese city</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/11/utol-focuses-on-driver-benefits-safety/</t>
+          <t>https://malaya.com.ph/news/international-news/blinken-urges-halt-to-middle-east-conflict-as-israel-bombs-historic-lebanese-city/</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="n">
-        <v>45576</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Smart supports proposal to remove Wi-Fi spectrum user fee</t>
+          <t>Britain, Germany sign new defense agreement as Ukraine tensions rise</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/11/smart-supports-proposal-to-remove-wi-fi-spectrum-user-fee/</t>
+          <t>https://malaya.com.ph/news/international-news/britain-germany-sign-new-defense-agreement-as-ukraine-tensions-rise/</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="n">
-        <v>45575</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Twilio unveils conversational AI applications</t>
+          <t>US says evidence shows North Korea has troops in Russia for Ukraine war</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/10/twilio-unveils-conversational-ai-applications/</t>
+          <t>https://malaya.com.ph/news/international-news/us-says-evidence-shows-north-korea-has-troops-in-russia-for-ukraine-war/</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="n">
-        <v>45575</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Smart, Maya warn customers against ‘text hijacking’</t>
+          <t>William Blake’s teenage copper plate doodles discovered</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/10/smart-maya-warn-customers-against-text-hijacking/</t>
+          <t>https://malaya.com.ph/living/arts/william-blakes-teenage-copper-plate-doodles-discovered/</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="n">
-        <v>45575</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ASEAN on track to 100% electrification, report says</t>
+          <t>Rockin’ Christmas</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/10/asean-on-track-to-100-electrification-report-says/</t>
+          <t>https://malaya.com.ph/living/rockin-christmas/</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="n">
-        <v>45574</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>AI startup raises $4.45m in new funding round</t>
+          <t>Award-winning designers explore sustainability</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/09/ai-startup-raises-4-45-in-new-funding-round/</t>
+          <t>https://malaya.com.ph/living/arts/award-winning-designers-explore-sustainability/</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="n">
-        <v>45574</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>What are brain-computer interfaces and how do they work?</t>
+          <t>Foundation adds the ‘Plus’ in health, livelihood initiatives</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/09/what-are-brain-computer-interfaces-and-how-do-they-work/</t>
+          <t>https://malaya.com.ph/living/foundation-adds-the-plus-in-health-livelihood-initiatives/</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="n">
-        <v>45574</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Globe commits to responsible AI maturity roadmap</t>
+          <t>Must-try activities at Metro’s premier wellness hub</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/09/globe-commits-to-responsible-ai-maturity-roadmap/</t>
+          <t>https://malaya.com.ph/living/health/must-try-activities-at-metros-premier-wellness-hub/</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="3" t="n">
-        <v>45573</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>INTERPOL cybercrime chief: ‘Don’t get hooked on social media’</t>
+          <t>New study rewrites decades of medical misunderstanding of saturated fat and heart disease</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/08/interpol-cybercrime-chief-dont-get-hooked-on-social-media/</t>
+          <t>https://malaya.com.ph/living/health/new-study-rewrites-decades-of-medical-misunderstanding-of-saturated-fat-and-heart-disease/</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="n">
-        <v>45573</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>DOJ says it will pursue suspect in Enzo Pastor case</t>
+          <t>Commitment to eliminate cervical cancer</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/08/doj-says-it-will-pursue-suspect-in-enzo-pastor-case/</t>
+          <t>https://malaya.com.ph/living/health/commitment-to-eliminate-cervical-cancer/</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="n">
-        <v>45572</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Travel review: HD Mountainville offers camping with a mountain view</t>
+          <t>Make your dream holiday trip happen with Mocasa</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/07/travel-review-hd-mountainville-offers-camping-with-a-mountain-view/</t>
+          <t>https://malaya.com.ph/living/make-your-dream-holiday-trip-happen-with-mocasa/</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="n">
-        <v>45572</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Philippine ITBPM sector seen hitting $38B in revenues</t>
+          <t>Maya, Landers roll out high-tech credit card</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/07/philippine-itbpm-sector-seen-hitting-38b-in-revenues/</t>
+          <t>https://malaya.com.ph/living/maya-landers-roll-out-high-tech-credit-card/</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="n">
-        <v>45571</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>First Look: Disney Adventure’s Imagination Garden</t>
+          <t>Hollywood stars hit the road for Harris</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/06/first-look-disney-adventures-imagination-garden/</t>
+          <t>https://malaya.com.ph/entertainment/hollywood-stars-hit-the-road-for-harris/</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="n">
-        <v>45570</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Eastern expands to Roxas City’s emerging digital hub</t>
+          <t>The Boss, Obama for Kamala; Hulk Hogan, Kid Rock for Trump</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/05/eastern-expands-to-roxas-citys-emerging-digital-hub/</t>
+          <t>https://malaya.com.ph/entertainment/the-boss-obama-for-kamala-hulk-hogan-kid-rock-for-trump/</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="n">
-        <v>45570</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Philippines opens manufacturing plant for EV battery component</t>
+          <t>All about loving oneself</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/05/philippines-opens-manufacturing-plant-for-ev-battery-component/</t>
+          <t>https://malaya.com.ph/entertainment/all-about-loving-oneself/</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="n">
-        <v>45569</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Philippines to host World Marketing Forum</t>
+          <t>‘Uninvited’ shakes up 50th MMFF with star-studded cast, crew</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/04/philippines-to-host-world-marketing-forum/</t>
+          <t>https://malaya.com.ph/entertainment/uninvited-shakes-up-50th-mmff-with-star-studded-cast-crew/</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="n">
-        <v>45569</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Jack Madrid speaks on impacts of AI</t>
+          <t>Pinky Webb leads ‘On Point’</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/04/jack-madrid-speaks-on-impacts-of-ai/</t>
+          <t>https://malaya.com.ph/entertainment/pinky-webb-leads-on-point/</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="n">
-        <v>45569</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Flying cars in the Philippines soon?</t>
+          <t>Jan Francis Alinsonorin shines at karaoke championship</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/04/flying-cars-in-the-philippines-soon/</t>
+          <t>https://malaya.com.ph/entertainment/music/jan-francis-alinsonorin-shines-at-karaoke-championship/</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="n">
-        <v>45569</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Agoda, tourism board join hands to showcase the Philippines</t>
+          <t>PHILIPPINE INTERNATIONAL MOTOR SHOW 2024: “Dare. Drive. The Future Redefined.” A peek into the future of Philippine mobility</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/04/agoda-tourism-board-join-hands-to-showcase-the-philippine/</t>
+          <t>https://malaya.com.ph/special-sections/philippine-international-motor-show-2024-dare-drive-the-future-redefined-a-peek-into-the-future-of-philippine-mobility/</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="3" t="n">
-        <v>45568</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Converge supports Kubota Philippines’ goal to sow seeds for the future</t>
+          <t>A brief history of the Philippine International Motor Show</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/03/converge-supports-kubota-philippines-goal-to-sow-seeds-for-the-future/</t>
+          <t>https://malaya.com.ph/special-sections/a-brief-history-of-the-philippine-international-motor-show/</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="3" t="n">
-        <v>45568</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>For MVP, it’s time to retire the word ‘digital’</t>
+          <t>Why the Mitsubishi booth is a must-visit at PIMS 2024</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/03/for-mvp-its-time-to-the-word-digital/</t>
+          <t>https://malaya.com.ph/special-sections/sponsored-content/why-the-mitsubishi-booth-is-a-must-visit-at-pims-2024/</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="3" t="n">
-        <v>45567</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>IC design competition crowns winners; honors industry pioneers</t>
+          <t>Chess match expected</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/02/ic-design-competition-crowns-winners-honors-industry-pioneers/</t>
+          <t>https://malaya.com.ph/sports/basketball/chess-match-expected/</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="n">
-        <v>45567</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>BuildHub PH partners with BPI to offer credit lines for construction firms</t>
+          <t>Zaragosa takes lead in brutal weather; rain halts play</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/02/buildhub-ph-partners-with-bpi-to-offer-credit-lines-for-construction-firms/</t>
+          <t>https://malaya.com.ph/sports/zaragosa-takes-lead-in-brutal-weather-rain-halts-play/</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="3" t="n">
-        <v>45566</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Tech firms unveil super app for pet owners</t>
+          <t>Fulfilling his late father’s wish</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/01/tech-firms-unveil-super-app-for-pet-owners/</t>
+          <t>https://malaya.com.ph/sports/fulfilling-his-late-fathers-wish/</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="3" t="n">
-        <v>45566</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Gushcloud unveils expansion plans, holds appreciation night</t>
+          <t>Abarrientos lives up to expectations</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://techtravelmonitor.com/2024/10/01/gushcloud-unveils-expansion-plans-holds-appreciation-night/</t>
+          <t>https://malaya.com.ph/sports/basketball/abarrientos-lives-up-to-expectations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Ababa stays ahead; tourney reduced to 36 holes</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/ababa-stays-ahead-tourney-reduced-to-36-holes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Cautious about being complacent</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/basketball/cautious-about-being-complacent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Making up for lost time, silly errors</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/basketball/making-up-for-lost-time-silly-errors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>‘It’s one of the greatest gifts I’ve ever got’</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/basketball/its-one-of-the-greatest-gifts-ive-ever-got/</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Editorial Cartoon</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/opinion-of-the-day/editorial-cartoon/editorial-cartoon-4/</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>For love of country: Kangleon 1944, Leyte patriots 2024</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/column-of-the-day/for-love-of-country-kangleon-1944-leyte-patriots-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Local salt for coconuts </t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/opinion-of-the-day/editorial-column/local-salt-for-coconuts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Biz group pushes strategies for growth</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/enterprise/biz-group-pushes-strategies-for-growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>IPOPHL seeks removal of Greenhills from notorious markets list</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/enterprise/ipophl-seeks-removal-of-greenhills-from-notorious-markets-list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>PEZA investments down but on track of target</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/enterprise/peza-investments-down-but-on-track-of-target/</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>PH eyes early conclusion of FTA negotiations with EU</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/enterprise/ph-eyes-early-conclusion-of-fta-negotiations-with-eu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8K operators to join PUV modernization</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/enterprise/8k-operators-to-join-puv-modernization/</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Stocks track Wall Street decline</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/enterprise/stocks-track-wall-street-decline/</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Four reforms to better serve developing countries pushed</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/four-reforms-to-better-serve-developing-countries-pushed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Palay output to drop in Q3</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/palay-output-to-drop-in-q3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>PLDT bags P2B loan to expand infra in underserved, unserved areas</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/pldt-bags-p2b-loan-to-expand-infra-in-underserved-unserved-areas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Gov’t to launch addl health projects</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/govt-to-launch-addl-health-projects/</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>MPIC, Keppel to divest from fuel terminal firm</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/mpic-keppel-to-divest-from-fuel-terminal-firm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>GPDRs eyed for offering by Q1, index futures by ’26</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/gpdrs-eyed-for-offering-by-q1-index-futures-by-26/</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Malampaya phase 4 secures EPNS certification </t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/malampaya-phase-4-secures-epns-certification/</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SM to open 87th mall </t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/sm-to-open-87th-mall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Small businesses to benefit from DOST-PCCI tech hub</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/small-businesses-to-benefit-from-dost-pcci-tech-hub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Global markets underestimating geopolitical risks, IMF says</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/international-business/global-markets-underestimating-geopolitical-risks-imf-says/</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>US economy remains engine of global growth, WEO says</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/international-business/us-economy-remains-engine-of-global-growth-weo-says/</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>S. Arabian economy to accelerate in 2025</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/international-business/s-arabian-economy-to-accelerate-in-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Gold hits record high on global uncertainties</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/international-business/gold-hits-record-high-on-global-uncertainties/</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Stocks climb</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/market/stocks-climb-27/</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Dollar soars</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/market/dollar-soars-2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>US-China ties to worsen slowly under Harris, exporters say</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/shipping-transportation/us-china-ties-to-worsen-slowly-under-harris-exporters-say/</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>EVs seen as a bumpy ride for battery metals</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/shipping-transportation/evs-seen-as-a-bumpy-ride-for-battery-metals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>LNG-fueled trucking accelerates in Asia</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/shipping-transportation/lng-fueled-trucking-accelerates-in-asia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Oil benchmarks slip</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/shipping-transportation/oil-benchmarks-slip-15/</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Shanghai aluminum up</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/shipping-transportation/shanghai-aluminum-up-2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Iron ore ticks down</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/shipping-transportation/iron-ore-ticks-down/</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Soybeans rise anew</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/shipping-transportation/soybeans-rise-anew/</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MMPC, SJ Legacy  expand presence in San Jose Del Monte </t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/mmpc-sj-legacy-expand-presence-in-san-jose-del-monte/</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Home Credit sees surge in iPhone sales</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/home-credit-sees-surge-in-iphone-sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IBAC director-general visits INAEC  </t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/ibac-director-general-visits-inaec/</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Toyota’s free vehicle safety inspection </t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/toyotas-free-vehicle-safety-inspection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PLDT, Smart engineers recount Batanes restoration  </t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/pldt-smart-engineers-recount-batanes-restoration/</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philips leads  smart home revolution  </t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/philips-leads-smart-home-revolution/</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BDO Travel Sale wraps up </t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/bdo-travel-sale-wraps-up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>PAL to move to new terminal at JFK airport in 2026</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate/pal-to-move-to-new-terminal-at-jfk-airport-in-2026/</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Concentrix Ph launches “Gadgets for Good”  </t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/concentrix-ph-launches-gadgets-for-good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>HONOR Magic7 Series to introduce Autopilot AI for Mobile</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/marketing-board/honor-magic7-series-to-introduce-autopilot-ai-for-mobile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>MR.DIY, Team Kramer bring ‘MERON DIYan! Caravan’ to Pampanga</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/marketing-board/mr-diy-team-kramer-bring-meron-diyan-caravan-to-pampanga/</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Media reps engage in interactive online purchase at Iskaparate.com’s press launch</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/marketing-board/media-reps-engage-in-interactive-online-purchase-at-iskaparate-coms-press-launch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Abalos pushes scrapping of amusement tax</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/entertainment/abalos-pushes-scrapping-of-amusement-tax/</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>October 24, 2024</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Painting the barangays through sports: MILO® and Boysen team up to support 200,000 Filipino kids</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/marketing-board/painting-the-barangays-through-sports-milo-and-boysen-team-up-to-support-200000-filipino-kids/</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Grade 9 student nabbed for illegal drugs in Taguig</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/grade-9-student-nabbed-for-illegal-drugs-in-taguig/</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Homepage – Malaya</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>PART 1 OF 2: MACHINE LEARNING FOR HUMAN-LIKE UNDERSTANDING: Will AI ever have an emotional quotient?</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/special-sections/part-1-of-2-machine-learning-for-human-like-understanding-will-ai-ever-have-an-emotional-quotient/</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Open access, collaboration needed as AI transforms infrastructure devt</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/special-sections/open-access-collaboration-needed-as-ai-transforms-infrastructure-devt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Instructure boosts mental wellness support with Microsoft</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/special-sections/instructure-boosts-mental-wellness-support-with-microsoft/</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Sophos acquires Secureworks</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/special-sections/sophos-acquires-secureworks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>OPPO Watch X is a true wellness companion</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/special-sections/oppo-watch-x-is-a-true-wellness-companion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>HONOR demonstrates Magic7 tricks with Autopilot, Snapdragon ecosystem</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/special-sections/honor-demonstrates-magic7-tricks-with-autopilot-snapdragon-ecosystem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Time to face the music,De Lima tells Duterte</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/time-to-face-the-musicde-lima-tells-duterte/</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Marcos dismisses Sara attacks</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/marcos-dismisses-sara-attacks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>‘Kristine’ intensifies; 47 areas under storm signal warnings</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/kristine-intensifies-47-areas-under-storm-signal-warnings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Legal actions eyed vs Chinese doing business as fake Pinoys</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/legal-actions-eyed-vs-chinese-doing-business-as-fake-pinoys/</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Courts OKs Quiboloy attendance in Senate hearing today</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/courts-oks-quiboloy-attendance-in-senate-hearing-today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>11.3M Pinoy families say they are poor</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/11-3m-pinoy-families-say-they-are-poor/</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>NAGKAISA slams ‘glaring disparity’ between NCR, provincial wage rates</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/nagkaisa-slams-glaring-disparity-between-ncr-provincial-wage-rates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>MMDA ramps up clearing operations for Undas</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/mmda-ramps-up-clearing-operations-for-undas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>P100K reward offered for info on kidnapped American vlogger</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/p100k-reward-offered-for-info-on-kidnapped-american-vlogger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>BuCor inaugurates 120-bed capacity hospital</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/bucor-inaugurates-120-bed-capacity-hospital/</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Proposed writ of kalayaan under review – SC chief</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/proposed-writ-of-kalayaan-under-review-sc-chief/</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Comelec warns bets: Register socmed accounts or face raps</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/comelec-warns-bets-register-socmed-accounts-or-face-raps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>2 Manila hospitals full but DOH raises no alarms</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/2-manila-hospitals-full-but-doh-raises-no-alarms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>17 more Pinoys back from Lebanon</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/17-more-pinoys-back-from-lebanon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Marcos lauds PCG for protecting PH</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/marcos-lauds-pcg-for-protecting-ph/</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Court OKs labor groups’ plea to intervene in PhilHealth case</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/court-oks-labor-groups-plea-to-intervene-in-philhealth-case/</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Trimming `top-heavy’ PNP: From 133 to just 25 generals</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/trimming-top-heavy-pnp-from-133-to-just-25-generals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Freeze order issued vs DQ of 3 local execs in ’25 polls</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/freeze-order-issued-vs-dq-of-3-local-execs-in-25-polls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Brian Poe: Championing animal rights and welfare</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/brian-poe-championing-animal-rights-and-welfare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Blinken in Israel in last big ceasefire push before US election</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/blinken-in-israel-in-last-big-ceasefire-push-before-us-election/</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>UN agency head calls for temporary truce in northern Gaza</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/un-agency-head-calls-for-temporary-truce-in-northern-gaza/</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Russian official says EU commits economic crime in giving Russian assets to Kyiv — TASS</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/russian-official-says-eu-commits-economic-crime-in-giving-russian-assets-to-kyiv-tass/</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Israel arrests seven Jerusalem residents over alleged Iran assassination plot</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/israel-arrests-seven-jerusalem-residents-over-alleged-iran-assassination-plot/</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>With polls tight, US election campaigns target overseas voters</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/with-polls-tight-us-election-campaigns-target-overseas-voters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Vatican, China extend deal over Catholic bishop appointments</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/news/vatican-china-extend-deal-over-catholic-bishop-appointments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Finding a foodie heaven in Tokyo Bay</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/food/finding-a-foodie-heaven-in-tokyo-bay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Celebrating 15 years with back-to-back Halloween treats</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/celebrating-15-yearswith-back-to-back-halloween-treats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Enjoy a meal and get a chance to fly to Dubai</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/food/enjoy-a-meal-and-get-a-chance-to-fly-to-dubai/</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>#Flavorfest returns as Wild West sauces meet Tropical Fruit Fizz drinks</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/food/flavorfest-returns-as-wild-west-sauces-meet-tropical-fruit-fizz-drinks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Celebrating super citizens during Elderly Filipino Week 2024</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/celebrating-super-citizens-during-elderly-filipino-week-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>New breakciting ‘Baon’ choice</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/new-breakciting-baon-choice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Next-generation Vaccines: a potential game-changer</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/next-generation-vaccines-a-potential-game-changer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>New research proves Centrum Silver Advance helps improve memory and mental sharpness</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/new-research-proves-centrum-silver-advance-helps-improve-memory-and-mental-sharpness/</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>CEU dominates Optomerists Licensure Exam with 7 topnotchers</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/ceu-dominates-optomerists-licensure-exam-with-7-topnotchers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Saving tips for Filipinos this holiday season with Wise</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/saving-tips-for-filipinos-this-holiday-season-with-wise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>EQ’s Maagang Pamasko E-Raffle</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/living/eqs-maagang-pamasko-e-raffle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Lionel Richie likens touring to vacation</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/entertainment/lionel-richie-likens-touring-to-vacation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Heartfelt homecoming</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/entertainment/heartfelt-homecoming/</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Heart to Pia: ‘Good luck’</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/showbiz/heart-to-pia-good-luck/</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>How Piolo stays in top shape</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/entertainment/how-piolo-stays-in-top-shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Streetboys stillin synch after 31 years</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/entertainment/streetboys-stillin-synch-after-31-years/</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>From ‘Dear SV’ to ‘Wil to Win’</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/entertainment/from-dear-sv-to-wil-to-win/</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Vice Ganda supports gig workers</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/entertainment/vice-ganda-supports-gig-workers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Proud parents </t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/entertainment/proud-parents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Star-studded showdown at MMFF 50</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/entertainment/star-studded-showdown-at-mmff-50/</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>They’re at it anew</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/basketball/theyre-at-it-anew/</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>UE tests resolve of UP quint</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/basketball/ue-tests-resolve-of-up-quint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Ababa rides rainy conditions, takes charge</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/ababa-rides-rainy-conditions-takes-charge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>NBA: Celtics have chip on their shoulders</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/basketball/nba-celtics-have-chip-on-their-shoulders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Resilient Bibat seizes ICTSI Negros lead</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/resilient-bibat-seizes-ictsi-negros-lead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Letran nips SSC, moves to solo 4th</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/basketball/letran-nips-ssc-moves-to-solo-4th/</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>World Dragon Boat tilt: Hopes high for Pinoy bets</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/world-dragon-boat-tilt-hopes-high-for-pinoy-bets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Mendoza bags elite title in Go For Gold race</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/sports/mendoza-bags-elite-title-in-go-for-gold-race/</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Editorial Cartoon</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/opinion-of-the-day/editorial-cartoon-3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Mistresses: Par for the course?</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/column-of-the-day/mistresses-par-for-the-course/</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>DOH’s tuberculosis treatment takes a backseat</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/column-of-the-day/dohs-tuberculosis-treatment-takes-a-backseat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Renewable energy projects </t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/opinion-of-the-day/renewable-energy-projects/</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>CONSUMER BASE LIFTS GROWTH: PH to outperform in region</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/consumer-base-lifts-growth-ph-to-outperform-in-region/</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Growth in RE supply highest in PH, but capacity lags</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/growth-in-re-supply-highest-in-ph-but-capacity-lags/</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Unified roadmap to fill housing gap</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/unified-roadmap-to-fill-housing-gap/</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>PH, Lao PDR to sign agriculture cooperation deal</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/ph-lao-pdr-to-sign-agriculture-cooperation-deal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Labor, environment pushed at FTA talks with EU</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/labor-environment-pushed-at-fta-talks-with-eu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Airfares stable in Nov</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/airfares-stable-in-nov/</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Cement supply sufficient; developers urged to buy local</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/cement-supply-sufficient-developers-urged-to-buy-local/</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Stocks up on cautious trade</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/stocks-up-on-cautious-trade-2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>AT NAIA: Technical glitch prompts early replacement of baggage handling</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/at-naia-technical-glitch-prompts-early-replacement-of-baggage-handling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>ICTSI enhances Melbourne operations</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/ictsi-enhances-melbourne-operations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>No new SRPs bulletin for rest of 2024: DTI</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/no-new-srps-bulletin-for-rest-of-2024-dti/</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>SMC completes acquisition of Bulacan water JVs</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/smc-completes-acquisition-of-bulacan-water-jvs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>The Bellagio Palawan to yield P3B</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/the-bellagio-palawan-to-yield-p3b/</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>RE developer eyes P2B solar power projects</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/re-developer-eyes-p2b-solar-power-projects/</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>PEZA seeks pharma investments</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/peza-seeks-pharma-investments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>China’s Q3 economic losses from natural calamities surge</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/chinas-q3-economic-losses-from-natural-calamities-surge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>IMF chief says higher prices are here to stay</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/imf-chief-says-higher-prices-are-here-to-stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Japan’s election outcome could muddle BOJ plans</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/japans-election-outcome-could-muddle-boj-plans/</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>4 Fed policy makers favor more rate cuts, but differ on pace</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/4-fed-policy-makers-favor-more-rate-cuts-but-differ-on-pace/</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Asia stocks end lower</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/market/asia-stocks-end-lower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Dollar strengthens</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/dollar-strengthens-49/</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Japan crude steel output falls anew</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/japan-crude-steel-output-falls-anew/</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Indonesia targets 1M hectares of new rice fields</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/indonesia-targets-1m-hectares-of-new-rice-fields/</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>AFTER GOVERNMENT ANNOUNCES TAX REVISION: Malaysian official says palm oil exporters ready</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/after-government-announces-tax-revision-malaysian-official-says-palm-oil-exporters-ready/</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>As US Permian crude turns lighter, it risks losing favor with refiners</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/as-us-permian-crude-turns-lighter-it-risks-losing-favor-with-refiners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Oil benchmarks dip</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/oil-benchmarks-dip-7/</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>London copper climbs</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/london-copper-climbs-5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Iron ore retreats</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/iron-ore-retreats-18/</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Soybeans, wheat ease</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/soybeans-wheat-ease-2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tanduay Asian Rum Silver wins gold  </t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/tanduay-asian-rum-silver-wins-gold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun meets functional  </t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/fun-meets-functional/</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Batangueño elderly become senior digizens  </t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/batangueno-elderly-become-senior-digizens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SAFC’s #BeALifeHero campaign  </t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/safcs-bealifehero-campaign/</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Distinguished panel ushers in the First Triple P Awards Winners</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/distinguished-panel-ushers-in-the-first-triple-p-awards-winners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 execs join leadership program on sustainability </t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/6-execs-join-leadership-program-on-sustainability/</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">USANA Ph at Circle of Excellence </t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/usana-ph-at-circle-of-excellence/</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EastWest Visa Platinum wins at The Asian Banker Awards  </t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/eastwest-visa-platinum-wins-at-the-asian-banker-awards/</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PLDT, Smart participate in Asean dialogues on child online protection </t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/corporate-roundup/pldt-smart-participate-in-asean-dialogues-on-child-online-protection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>SM, DENR partner to save critically endangered PHL species</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/business-news/sm-denr-partner-to-save-critically-endangered-phl-species/</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Seamless transition between study and play with realme 13 series 5G</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/marketing-board/seamless-transition-between-study-and-play-with-realme-13-series-5g/</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Japan Agenda: The Premium Travel Blueprint</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/marketing-board/japan-agenda-the-premium-travel-blueprint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Handover ceremony for ASPIRE BARMM project in Basilan</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/marketing-board/handover-ceremony-for-aspire-barmm-project-in-basilan/</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>October 23, 2024</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>JA Philippines launches ‘Your Global Edge’</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>https://malaya.com.ph/marketing-board/ja-philippines-launches-your-global-edge/</t>
         </is>
       </c>
     </row>
@@ -1288,6 +4057,163 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C51" r:id="rId50"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C52" r:id="rId51"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C53" r:id="rId52"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId53"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId54"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId55"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C57" r:id="rId56"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C58" r:id="rId57"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C59" r:id="rId58"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C60" r:id="rId59"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C61" r:id="rId60"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C62" r:id="rId61"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C63" r:id="rId62"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C64" r:id="rId63"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C65" r:id="rId64"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C66" r:id="rId65"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C67" r:id="rId66"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C68" r:id="rId67"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C69" r:id="rId68"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C70" r:id="rId69"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C71" r:id="rId70"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C72" r:id="rId71"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C73" r:id="rId72"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C74" r:id="rId73"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C75" r:id="rId74"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C76" r:id="rId75"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C77" r:id="rId76"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C78" r:id="rId77"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C79" r:id="rId78"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C80" r:id="rId79"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C81" r:id="rId80"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C82" r:id="rId81"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C83" r:id="rId82"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C84" r:id="rId83"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C85" r:id="rId84"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C86" r:id="rId85"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C87" r:id="rId86"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C88" r:id="rId87"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C89" r:id="rId88"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C90" r:id="rId89"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C91" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C92" r:id="rId91"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C93" r:id="rId92"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C94" r:id="rId93"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C95" r:id="rId94"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C96" r:id="rId95"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C97" r:id="rId96"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C98" r:id="rId97"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C99" r:id="rId98"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C100" r:id="rId99"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C101" r:id="rId100"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C102" r:id="rId101"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C103" r:id="rId102"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C104" r:id="rId103"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C105" r:id="rId104"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C106" r:id="rId105"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C107" r:id="rId106"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C108" r:id="rId107"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C109" r:id="rId108"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C110" r:id="rId109"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C111" r:id="rId110"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C112" r:id="rId111"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C113" r:id="rId112"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C114" r:id="rId113"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C115" r:id="rId114"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C116" r:id="rId115"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C117" r:id="rId116"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C118" r:id="rId117"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C119" r:id="rId118"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C120" r:id="rId119"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C121" r:id="rId120"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C122" r:id="rId121"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C123" r:id="rId122"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C124" r:id="rId123"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C125" r:id="rId124"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C126" r:id="rId125"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C127" r:id="rId126"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C128" r:id="rId127"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C129" r:id="rId128"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C130" r:id="rId129"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C131" r:id="rId130"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C132" r:id="rId131"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C133" r:id="rId132"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C134" r:id="rId133"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C135" r:id="rId134"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C136" r:id="rId135"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C137" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C138" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C139" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C140" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C141" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C142" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C143" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C144" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C145" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C146" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C147" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C148" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C149" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C150" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C151" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C152" r:id="rId151"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C153" r:id="rId152"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C154" r:id="rId153"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C155" r:id="rId154"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C156" r:id="rId155"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C157" r:id="rId156"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C158" r:id="rId157"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C159" r:id="rId158"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C160" r:id="rId159"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C161" r:id="rId160"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C162" r:id="rId161"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C163" r:id="rId162"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C164" r:id="rId163"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C165" r:id="rId164"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C166" r:id="rId165"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C167" r:id="rId166"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C168" r:id="rId167"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C169" r:id="rId168"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C170" r:id="rId169"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C171" r:id="rId170"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C172" r:id="rId171"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C173" r:id="rId172"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C174" r:id="rId173"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C175" r:id="rId174"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C176" r:id="rId175"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C177" r:id="rId176"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C178" r:id="rId177"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C179" r:id="rId178"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C180" r:id="rId179"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C181" r:id="rId180"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C182" r:id="rId181"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C183" r:id="rId182"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C184" r:id="rId183"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C185" r:id="rId184"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C186" r:id="rId185"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C187" r:id="rId186"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C188" r:id="rId187"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C189" r:id="rId188"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C190" r:id="rId189"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C191" r:id="rId190"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C192" r:id="rId191"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C193" r:id="rId192"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C194" r:id="rId193"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C195" r:id="rId194"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C196" r:id="rId195"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C197" r:id="rId196"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C198" r:id="rId197"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C199" r:id="rId198"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C200" r:id="rId199"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C201" r:id="rId200"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C202" r:id="rId201"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C203" r:id="rId202"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C204" r:id="rId203"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C205" r:id="rId204"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C206" r:id="rId205"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C207" r:id="rId206"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C208" r:id="rId207"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C209" r:id="rId208"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C210" r:id="rId209"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added delay on request
</commit_message>
<xml_diff>
--- a/pages/fetcher_temp/temp.xlsx
+++ b/pages/fetcher_temp/temp.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,647 +456,436 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>45589</v>
+        <v>45687</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    See Through Luxury with Porsche's Eyewear Collection
-  </t>
+          <t>Leveling up: Willy Ocier’s LOTO confirms entry into high-stakes digital gaming</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/see-through-luxury-with-porsches-eyewear-collection</t>
+          <t>https://bilyonaryo.com/2025/01/30/leveling-up-willy-ociers-loto-confirms-entry-into-high-stakes-digital-gaming/business/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>45589</v>
+        <v>45687</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    HALA: Cebu’s Art &amp; Design Folio
-  </t>
+          <t>New leadership, new vision: EJ Qua Hiansen’s big plans for FINEX</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/hala-cebus-art-amp-design-folio</t>
+          <t>https://bilyonaryo.com/2025/01/30/new-leadership-new-vision-ej-qua-hiansens-big-plans-for-finex/business/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>45589</v>
+        <v>45687</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Where East Meets West: Louvre Abu Dhabi
-  </t>
+          <t>The pioneering science linking climate to weather disasters</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/where-east-meets-west-louvre-abu-dhabi</t>
+          <t>https://bilyonaryo.com/2025/01/30/the-pioneering-science-linking-climate-to-weather-disasters/weather/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>45588</v>
+        <v>45687</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Beyond Shores: Designing the Future at Design Week Philippines
-  </t>
+          <t>Air freight rose to record levels in 2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/beyond-shores-designing-the-future-at-design-week-philippines</t>
+          <t>https://bilyonaryo.com/2025/01/30/air-freight-rose-to-record-levels-in-2024/travel/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>45588</v>
+        <v>45687</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Boggi Milano Opens Its Flagship Store in Greenbelt 5, Makati City Philippines
-  </t>
+          <t>‘Very sad’ west Londoners oppose Heathrow expansion</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/boggi-milano-opens-its-flagship-store-in-greenbelt-5-makati-city-philippines</t>
+          <t>https://bilyonaryo.com/2025/01/30/very-sad-west-londoners-oppose-heathrow-expansion/infrastructure/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>45588</v>
+        <v>45687</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    What’s New with the G-SHOCK GM-2110D Series?
-  </t>
+          <t>Maison Margiela names new lead designer during Paris Haute Couture Week</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/whats-new-with-the-g-shock-gm-2110d-series</t>
+          <t>https://bilyonaryo.com/2025/01/30/maison-margiela-names-new-lead-designer-during-paris-haute-couture-week/lifestyle/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>45588</v>
+        <v>45687</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    This Hidden Café in Cavite is an Instagrammable Hot Spot
-  </t>
+          <t>Harvey Weinstein seeks early retrial over ‘hellhole’ prison conditions</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/this-hidden-caf-in-cavite-is-an-instagrammable-hot-spot</t>
+          <t>https://bilyonaryo.com/2025/01/30/harvey-weinstein-seeks-early-retrial-over-hellhole-prison-conditions/entertainment/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>45588</v>
+        <v>45687</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Merging Distinct Styles: The CC x LL Exhibition
-  </t>
+          <t>Meta posts big profit, aims to take AI lead</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/merging-distinct-styles-the-cc-x-ll-exhibition</t>
+          <t>https://bilyonaryo.com/2025/01/30/meta-posts-big-profit-aims-to-take-ai-lead/technology/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>45588</v>
+        <v>45687</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Jonathan Ching Paints the Many Colors Between Life and Death
-  </t>
+          <t>Price tag reaches $8M for Super Bowl LIX commercials</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/jonathan-ching-paints-the-many-colors-between-life-and-death</t>
+          <t>https://bilyonaryo.com/2025/01/30/price-tag-reaches-8m-for-super-bowl-lix-commercials/sports/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>45587</v>
+        <v>45687</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Clear Focus on Southeast Asia
-  </t>
+          <t>Tiger-Rory showdown fails to bring TGL big ratings boost</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/clear-focus-on-southeast-asia</t>
+          <t>https://bilyonaryo.com/2025/01/30/tiger-rory-showdown-fails-to-bring-tgl-big-ratings-boost/golf/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>45587</v>
+        <v>45687</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    The Magic Formula Behind What Really Makes Art Worth Millions
-  </t>
+          <t>Microsoft rolls out DeepSeek’s AI model on Azure</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/column-art-nomad</t>
+          <t>https://bilyonaryo.com/2025/01/30/microsoft-rolls-out-deepseeks-ai-model-on-azure/technology/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>45586</v>
+        <v>45687</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    An Art Affair
-  </t>
+          <t>New York says 1 million fewer vehicles have entered Manhattan since congestion pricing start</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/an-art-affair</t>
+          <t>https://bilyonaryo.com/2025/01/30/new-york-says-1-million-fewer-vehicles-have-entered-manhattan-since-congestion-pricing-start/mobility/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>45586</v>
+        <v>45687</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    PIID at 60: A Legacy of Design Excellence
-  </t>
+          <t>Vodafone makes world’s first satellite video call using standard smartphone</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/piid-at-60-a-legacy-of-design-excellence4o</t>
+          <t>https://bilyonaryo.com/2025/01/30/vodafone-makes-worlds-first-satellite-video-call-using-standard-smartphone/technology/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>45586</v>
+        <v>45687</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Pic at the Beau-Rivage Palace
-  </t>
+          <t>Fed leaves rates unchanged, sees no hurry to cut again</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/pic-at-the-beau-rivage-palace</t>
+          <t>https://bilyonaryo.com/2025/01/30/fed-leaves-rates-unchanged-sees-no-hurry-to-cut-again/money/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>45583</v>
+        <v>45687</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Time Distilled: The Black and - White Hyperrealism of Arnold Lalongisip
-  </t>
+          <t>Renee Zellweger celebrates ‘old friend’ Bridget Jones as film has London premiere</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/timenbsp-distilled-the-black-and-white-hyperrealism-of-arnold-lalongisip</t>
+          <t>https://bilyonaryo.com/2025/01/30/renee-zellweger-celebrates-old-friend-bridget-jones-as-film-has-london-premiere/entertainment/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>45582</v>
+        <v>45687</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    The Little that is Left
-  </t>
+          <t>Tesla commits to cheaper cars in first half, sees autonomous vehicles ‘in the wild’ soon</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/the-little-that-is-left</t>
+          <t>https://bilyonaryo.com/2025/01/30/tesla-commits-to-cheaper-cars-in-first-half-sees-autonomous-vehicles-in-the-wild-soon/mobility/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>45581</v>
+        <v>45687</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Get Khozy in Massage MNL's New Physical Branch at Makati
-  </t>
+          <t>Viktor Hovland aims to rediscover his game at Pebble Beach</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/get-khozy-in-massage-mnls-new-physical-branch-at-makati</t>
+          <t>https://bilyonaryo.com/2025/01/30/viktor-hovland-aims-to-rediscover-his-game-at-pebble-beach/golf/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>45581</v>
+        <v>45687</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Visit This Italian Villa That’s Only 1 Hour Away from Metro Manila
-  </t>
+          <t>Theft and violence in UK retail soar to record levels, survey shows</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/visit-this-italian-villa-thats-only-1-hour-away-from-metro-manila</t>
+          <t>https://bilyonaryo.com/2025/01/30/theft-and-violence-in-uk-retail-soar-to-record-levels-survey-shows/retail/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
-        <v>45581</v>
+        <v>45687</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Healing through Sound
-  </t>
+          <t>Nestle to invest $1 billion in Mexico operations over three years</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/healing-through-sound</t>
+          <t>https://bilyonaryo.com/2025/01/30/nestle-to-invest-1-billion-in-mexico-operations-over-three-years/food/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>45581</v>
+        <v>45687</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Bar Boys: A New Musical makes a powerful comeback
-  </t>
+          <t>Sony names new CEO in management reshuffle</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/bar-boys-a-new-musical-makes-a-powerful-comeback</t>
+          <t>https://bilyonaryo.com/2025/01/30/sony-names-new-ceo-in-management-reshuffle/technology/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
-        <v>45581</v>
+        <v>45687</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Newport World Resorts brings “Gags for Days!”
-  </t>
+          <t>Dead Sea an ‘ecological disaster’, but no one can agree how to fix it</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/newport-world-resorts-brings-gags-for-days</t>
+          <t>https://bilyonaryo.com/2025/01/30/dead-sea-an-ecological-disaster-but-no-one-can-agree-how-to-fix-it/nature/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n">
-        <v>45580</v>
+        <v>45687</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Runway Recap: Here's What You Missed Out on in BYS Fashion Week '24
-  </t>
+          <t>Fears of scam center kidnaps keep Chinese tourists on edge in Thailand</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/runway-recap-heres-what-you-missed-out-on-in-bys-fashion-week-24</t>
+          <t>https://bilyonaryo.com/2025/01/30/fears-of-scam-center-kidnaps-keep-chinese-tourists-on-edge-in-thailand/scams/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
-        <v>45580</v>
+        <v>45687</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Breaking the Fifth Wall
-  </t>
+          <t>Europe torn between bigger airports and climate goals</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/breaking-the-fifth-wall</t>
+          <t>https://bilyonaryo.com/2025/01/30/europe-torn-between-bigger-airports-and-climate-goals/nature/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="n">
-        <v>45580</v>
+        <v>45687</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    There’s Always a Silver Lining
-  </t>
+          <t>At least 30 dead in India stampede at Hindu mega-festival</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/theres-always-a-silver-lining</t>
+          <t>https://bilyonaryo.com/2025/01/30/at-least-30-dead-in-india-stampede-at-hindu-mega-festival/lifestyle/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="n">
-        <v>45580</v>
+        <v>45686</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Building an Ecosystem
-  </t>
+          <t>Czech central bank to consider holding bitcoin as reserve asset</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/building-an-ecosystem</t>
+          <t>https://bilyonaryo.com/2025/01/30/czech-central-bank-to-consider-holding-bitcoin-as-reserve-asset/money/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="n">
-        <v>45579</v>
+        <v>45686</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Q&amp;A with Lea Salonga on Request sa Radyo
-  </t>
+          <t>A fresh property for Makati’s elite: Radisson to open luxury serviced apartments by 2026</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/qampa-with-lea-salonga-on-request-sa-radyo</t>
+          <t>https://bilyonaryo.com/2025/01/30/a-fresh-property-for-makatis-elite-radisson-to-open-luxury-serviced-apartments-by-2026/property/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="n">
-        <v>45576</v>
+        <v>45686</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Slice of Life: A Review of Request sa Radyo
-  </t>
+          <t>EU points way to competitive future to catch US, China rivals</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/slice-of-life-a-review-of-request-sa-radyo</t>
+          <t>https://bilyonaryo.com/2025/01/30/eu-points-way-to-competitive-future-to-catch-us-china-rivals/trade/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="n">
-        <v>45576</v>
+        <v>45686</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Reimagining Filipino Folklore in REP’s Jepoy and the Magic Circle
-  </t>
+          <t>Tech reboot lifts European stocks to record high ahead of Fed meeting</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/reimagining-filipino-folklore-in-reps-jepoy-and-the-magic-circle</t>
+          <t>https://bilyonaryo.com/2025/01/30/tech-reboot-lifts-european-stocks-to-record-high-ahead-of-fed-meeting/money/</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="n">
-        <v>45575</v>
+        <v>45686</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-    Our 5 Must-Visit Spots for Museums and Galleries Month
-  </t>
+          <t>UK’s Princess Beatrice gives birth to second baby girl</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://artplus.squarespace.com/features/our-5-must-visit-spots-for-museums-and-galleries-month</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="3" t="n">
-        <v>45574</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-    Boracay Island Flavors: A Culinary Journey at Savoy Hotel Manila
-  </t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>https://artplus.squarespace.com/features/boracay-island-flavors-a-culinary-journey-at-savoy-hotel-manila</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="3" t="n">
-        <v>45573</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-    This Shirt Collection Celebrates Worldwide Peace for All Humanity
-  </t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>https://artplus.squarespace.com/features/this-shirt-collection-celebrates-worldwide-peace-for-all-humanity</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="n">
-        <v>45569</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-     160 Years With Perrier and Its Art
-  </t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>https://artplus.squarespace.com/features/nbsp160-years-with-perrier-and-its-art</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="n">
-        <v>45569</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-    Situ: Where Performance Takes an Art Form
-  </t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>https://artplus.squarespace.com/features/situ-where-performance-takes-an-art-form</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="3" t="n">
-        <v>45569</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-    These 5 Filipinas Graced Paris Fashion Week 2024
-  </t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>https://artplus.squarespace.com/features/these-5-filipinas-graced-paris-fashion-week-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="3" t="n">
-        <v>45569</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-    Look: Australia's St. Ali Coffee is Officially in the Philippines
-  </t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>https://artplus.squarespace.com/features/look-australias-st-ali-coffee-is-officially-in-the-philippines</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="3" t="n">
-        <v>45567</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-    “MUSIC, MOVIES, MAGIC”
-  </t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>https://artplus.squarespace.com/features/music-movies-magic</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="3" t="n">
-        <v>45566</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-    Provocation and Evocation: Exhibits in September 2024
-  </t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>https://artplus.squarespace.com/features/provocation-and-evocation-exhibits-in-september-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="3" t="n">
-        <v>45566</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-    5 Affordable Alba Watches for the Young Professional
-  </t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>https://artplus.squarespace.com/features/5-affordable-alba-watches-for-the-young-professional</t>
+          <t>https://bilyonaryo.com/2025/01/30/uks-princess-beatrice-gives-birth-to-second-baby-girl/lifestyle/</t>
         </is>
       </c>
     </row>
@@ -1131,15 +920,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C28" r:id="rId27"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C29" r:id="rId28"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C30" r:id="rId29"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C31" r:id="rId30"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C32" r:id="rId31"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C33" r:id="rId32"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C34" r:id="rId33"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C35" r:id="rId34"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C36" r:id="rId35"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C37" r:id="rId36"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C38" r:id="rId37"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C39" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>